<commit_message>
LuLa: update regarding alignment
</commit_message>
<xml_diff>
--- a/agenda/agenda_21_03.xlsx
+++ b/agenda/agenda_21_03.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="111">
   <si>
     <t>sphero</t>
   </si>
@@ -27,10 +27,6 @@
   </si>
   <si>
     <t>Koordynator:</t>
-  </si>
-  <si>
-    <t>sphero, 
-przerywniki</t>
   </si>
   <si>
     <t>robogames, 
@@ -273,12 +269,6 @@
     <t>Marek P.</t>
   </si>
   <si>
-    <t>Piotrek K.</t>
-  </si>
-  <si>
-    <t>Kasia/Zuza</t>
-  </si>
-  <si>
     <t>Org.</t>
   </si>
   <si>
@@ -327,7 +317,45 @@
     <t>LEGO (tempomat)</t>
   </si>
   <si>
-    <t>LEGO (LeOS - na 2.0)</t>
+    <t>LEGO (LeJOS - na 2.0)</t>
+  </si>
+  <si>
+    <t>sphero, 
+przerywniki,
+LEGO (2.0)</t>
+  </si>
+  <si>
+    <t>Marcin, Lukasz G.</t>
+  </si>
+  <si>
+    <t>Zuza, Jacek</t>
+  </si>
+  <si>
+    <t>Jacek, Krzychu</t>
+  </si>
+  <si>
+    <t>Marcin, Lukasz L</t>
+  </si>
+  <si>
+    <t>Piotrek K., Krzychu</t>
+  </si>
+  <si>
+    <t>Marek P., Piotrek S.</t>
+  </si>
+  <si>
+    <t>Piotrek K., Marek P.</t>
+  </si>
+  <si>
+    <t>Lukasz L, Marek P.</t>
+  </si>
+  <si>
+    <t>Zuza, Lukasz G.</t>
+  </si>
+  <si>
+    <t>Kasia/Piotrek S./Ala</t>
+  </si>
+  <si>
+    <t>Zuza,  Lukasz L</t>
   </si>
 </sst>
 </file>
@@ -388,7 +416,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,6 +460,12 @@
         <fgColor theme="7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -452,7 +486,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
@@ -476,6 +510,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="8" borderId="0" xfId="7" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -777,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -791,7 +826,7 @@
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
     <col min="8" max="8" width="22.140625" customWidth="1"/>
     <col min="9" max="9" width="21.28515625" customWidth="1"/>
     <col min="10" max="10" width="23" customWidth="1"/>
@@ -802,40 +837,40 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1"/>
       <c r="L1" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -850,31 +885,39 @@
     <row r="3" spans="1:13" ht="74.25" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="G3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="I3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J3" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="14.25" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -888,31 +931,39 @@
     <row r="5" spans="1:13" ht="75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G5" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H5" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="I5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="3" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="32.25" customHeight="1">
       <c r="A6" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -926,31 +977,39 @@
     <row r="7" spans="1:13" ht="78.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="E7" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="G7" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H7" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="I7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="24" customHeight="1">
       <c r="A8" s="12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -963,60 +1022,55 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="B12" t="s">
+    <row r="13" spans="1:13">
+      <c r="B13" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="B14" s="15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="B14" t="s">
+    <row r="15" spans="1:13">
+      <c r="B15" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
-      <c r="B15" t="s">
+    <row r="16" spans="1:13">
+      <c r="B16" s="15" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="B16" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
-        <v>82</v>
-      </c>
-    </row>
     <row r="19" spans="2:2">
-      <c r="B19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
-        <v>8</v>
+      <c r="B19" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1043,289 +1097,289 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
-        <v>28</v>
-      </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="45">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30">
       <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
         <v>59</v>
       </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>